<commit_message>
__describe checkbox "Lưu lại kết quả sắp xếp lần này" on GUI_003(sort) CommonFunctionGui.xlsx
</commit_message>
<xml_diff>
--- a/Specifications/CommonFunctionGui.xlsx
+++ b/Specifications/CommonFunctionGui.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GUI_001" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Màn hình:</t>
   </si>
@@ -165,8 +165,40 @@
     <t>Tìm kiếm dữ liệu trên database dựa theo các điều kiện search, màn hình tìm kiếm close, dữ liệu trên màn hình Output là dữ liệu tìm kiếm được</t>
   </si>
   <si>
+    <t>Sắp xếp nâng cao</t>
+  </si>
+  <si>
+    <t>Nhấn Add Formula</t>
+  </si>
+  <si>
+    <t>Chức năng  lưu lại kết quả sắp sếp lần này.</t>
+  </si>
+  <si>
+    <t>Checkbox "Lưu lại kết quả sắp xếp lần này".</t>
+  </si>
+  <si>
+    <t>Nếu ko check thì ko ảnh hưởng gì cả.</t>
+  </si>
+  <si>
+    <t>Nếu có check, thì Kết quả sắp xếp, theo điều kiện đã chọn, trong lần sắp xếp này, sẽ được lưu lại.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tức là mỗi khi mở màn hình này lên, thì dữ liệu hiển thị ra đã được sắp xếp theo điều kiện sort trước đó, chứ ko phải là sắp xếp dữ liệu theo code mặc định. </t>
+  </si>
+  <si>
+    <t>Ví dụ ta đang ở màn hình Khách hàng và trong màn hình Khách hàng này có nút sort.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ta click vào nút sort và chọn điều kiện 1 là sort theo tên khách hàng, điều kiện 2 là sort theo ngày tháng năm sinh, và ta để trống điều kiện 3 và điều kiện 4, và ta có check vào checkbox "lưu lại kết quả sắp xếp lần này" và nhấn nút OK (hay gọi là nút "Sắp xếp"), sau đó màn hình khách hàng sẽ hiện ra các dòng dữ liệu được sort theo thứ tự Tên khách hàng và ngày tháng năm sinh. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Và kết quả sort này sẽ được lưu lại mỗi khi ta mở form khách hàng này lên. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trước đó form khách hàng này được code mặc định là sort theo mã số khách hàng mỗi khi được mở lên, giờ đây thì đã bị thay đổi. </t>
+  </si>
+  <si>
     <t>Dữ liệu output sẽ được sắp sếp theo 4 KEY</t>
-    <phoneticPr fontId="0"/>
   </si>
 </sst>
 </file>
@@ -214,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -223,6 +255,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,8 +479,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>458408</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>134060</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38810</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -484,8 +517,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>410781</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>38788</xdr:rowOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>114988</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -522,8 +555,8 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>458413</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>162630</xdr:rowOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>57855</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -542,6 +575,82 @@
         <a:xfrm>
           <a:off x="600075" y="11944350"/>
           <a:ext cx="7659313" cy="5048955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>144172</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>10133</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="sortnangcao.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="19050000"/>
+          <a:ext cx="9288172" cy="4353533"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>201160</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>19634</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="1.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="24003000"/>
+          <a:ext cx="8125960" cy="4182059"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -955,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3307,13 +3416,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:N130"/>
+  <dimension ref="A3:N160"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L101" sqref="L101"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="E164" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="4"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:14">
       <c r="A3" s="1"/>
@@ -3334,7 +3446,7 @@
     <row r="4" spans="1:14">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -4855,7 +4967,9 @@
     </row>
     <row r="99" spans="1:14">
       <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
+      <c r="B99" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -5271,7 +5385,9 @@
     </row>
     <row r="125" spans="1:14">
       <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
+      <c r="B125" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
@@ -5365,8 +5481,54 @@
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
     </row>
+    <row r="151" spans="2:2">
+      <c r="B151" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2">
+      <c r="B153" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2">
+      <c r="B154" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2">
+      <c r="B155" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2">
+      <c r="B156" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2">
+      <c r="B157" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2">
+      <c r="B158" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2">
+      <c r="B159" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2">
+      <c r="B160" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>